<commit_message>
working on joint mdl test data
</commit_message>
<xml_diff>
--- a/data/rmblTraitData.xlsx
+++ b/data/rmblTraitData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/Treetraits/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61E3D21-51E7-4944-A5E7-00BA2D45261B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B1B2E6-4DC0-3749-965B-454FC2125D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="24340" windowHeight="16120" activeTab="1" xr2:uid="{C96981F3-3DE4-AD4D-83E7-94579CDCB6C4}"/>
+    <workbookView xWindow="-34020" yWindow="460" windowWidth="24340" windowHeight="16080" activeTab="1" xr2:uid="{C96981F3-3DE4-AD4D-83E7-94579CDCB6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="scratch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5488" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5561" uniqueCount="64">
   <si>
     <t>site</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>20B</t>
+  </si>
+  <si>
+    <t>Mertensia f</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6055DB2-DEED-8741-98AF-46EB041D164E}">
   <dimension ref="A1:K138"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
@@ -5031,6 +5034,12 @@
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" t="s">
+        <v>30</v>
+      </c>
       <c r="C135">
         <v>2</v>
       </c>
@@ -5060,6 +5069,12 @@
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" t="s">
+        <v>30</v>
+      </c>
       <c r="C136">
         <v>3</v>
       </c>
@@ -5089,6 +5104,12 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>18</v>
+      </c>
+      <c r="B137" t="s">
+        <v>30</v>
+      </c>
       <c r="C137">
         <v>4</v>
       </c>
@@ -5118,6 +5139,12 @@
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" t="s">
+        <v>30</v>
+      </c>
       <c r="C138">
         <v>5</v>
       </c>
@@ -5155,8 +5182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0085D955-7D43-4D44-91E1-7EE929C3D60B}">
   <dimension ref="A1:K1729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" workbookViewId="0">
-      <selection activeCell="F1709" sqref="F1709"/>
+    <sheetView tabSelected="1" topLeftCell="A1705" workbookViewId="0">
+      <selection activeCell="J1714" sqref="J1714:J1715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -43562,7 +43589,7 @@
         <v>14</v>
       </c>
       <c r="F1680">
-        <v>0.19746</v>
+        <v>8.3919999999999995E-2</v>
       </c>
       <c r="G1680">
         <v>3.8490000000000002</v>
@@ -43571,7 +43598,13 @@
         <v>1.7229999999999999E-2</v>
       </c>
     </row>
-    <row r="1681" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1681" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1681" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1681" t="s">
+        <v>23</v>
+      </c>
       <c r="D1681" s="6">
         <v>1</v>
       </c>
@@ -43588,7 +43621,13 @@
         <v>2.4649999999999998E-2</v>
       </c>
     </row>
-    <row r="1682" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1682" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1682" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1682" t="s">
+        <v>23</v>
+      </c>
       <c r="D1682" s="6">
         <v>2</v>
       </c>
@@ -43605,7 +43644,13 @@
         <v>2.7699999999999999E-2</v>
       </c>
     </row>
-    <row r="1683" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1683" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1683" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1683" t="s">
+        <v>23</v>
+      </c>
       <c r="D1683" s="6">
         <v>2</v>
       </c>
@@ -43622,7 +43667,13 @@
         <v>3.7719999999999997E-2</v>
       </c>
     </row>
-    <row r="1684" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1684" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1684" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1684" t="s">
+        <v>23</v>
+      </c>
       <c r="D1684" s="6">
         <v>3</v>
       </c>
@@ -43639,7 +43690,13 @@
         <v>1.0829999999999999E-2</v>
       </c>
     </row>
-    <row r="1685" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1685" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1685" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1685" t="s">
+        <v>23</v>
+      </c>
       <c r="D1685" s="6">
         <v>3</v>
       </c>
@@ -43656,7 +43713,13 @@
         <v>1.6150000000000001E-2</v>
       </c>
     </row>
-    <row r="1686" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1686" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1686" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1686" t="s">
+        <v>23</v>
+      </c>
       <c r="D1686" s="6">
         <v>4</v>
       </c>
@@ -43673,7 +43736,13 @@
         <v>2.4379999999999999E-2</v>
       </c>
     </row>
-    <row r="1687" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1687" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1687" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1687" t="s">
+        <v>23</v>
+      </c>
       <c r="D1687" s="6">
         <v>4</v>
       </c>
@@ -43690,7 +43759,13 @@
         <v>2.0039999999999999E-2</v>
       </c>
     </row>
-    <row r="1688" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="1688" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1688" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1688" t="s">
+        <v>23</v>
+      </c>
       <c r="D1688" s="6">
         <v>5</v>
       </c>
@@ -43700,8 +43775,20 @@
       <c r="F1688">
         <v>0.1091</v>
       </c>
-    </row>
-    <row r="1689" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1688">
+        <v>4.8479999999999999</v>
+      </c>
+      <c r="H1688">
+        <v>2.2749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1689" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1689" t="s">
+        <v>23</v>
+      </c>
       <c r="D1689" s="6">
         <v>5</v>
       </c>
@@ -43711,8 +43798,20 @@
       <c r="F1689">
         <v>9.0660000000000004E-2</v>
       </c>
-    </row>
-    <row r="1690" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1689">
+        <v>4.2709999999999999</v>
+      </c>
+      <c r="H1689">
+        <v>1.9699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1690" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1690" t="s">
+        <v>31</v>
+      </c>
       <c r="D1690" s="6">
         <v>1</v>
       </c>
@@ -43722,8 +43821,20 @@
       <c r="F1690">
         <v>1.804E-2</v>
       </c>
-    </row>
-    <row r="1691" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1690">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="H1690">
+        <v>2.7599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1691" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1691" t="s">
+        <v>31</v>
+      </c>
       <c r="D1691" s="6">
         <v>1</v>
       </c>
@@ -43733,8 +43844,20 @@
       <c r="F1691">
         <v>1.524E-2</v>
       </c>
-    </row>
-    <row r="1692" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1691">
+        <v>0.438</v>
+      </c>
+      <c r="H1691">
+        <v>2.6199999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1692" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1692" t="s">
+        <v>31</v>
+      </c>
       <c r="D1692" s="6">
         <v>2</v>
       </c>
@@ -43744,8 +43867,20 @@
       <c r="F1692">
         <v>2.2200000000000001E-2</v>
       </c>
-    </row>
-    <row r="1693" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1692">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H1692">
+        <v>4.1200000000000004E-3</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1693" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1693" t="s">
+        <v>31</v>
+      </c>
       <c r="D1693" s="6">
         <v>2</v>
       </c>
@@ -43755,8 +43890,20 @@
       <c r="F1693">
         <v>2.9960000000000001E-2</v>
       </c>
-    </row>
-    <row r="1694" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1693">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="H1693">
+        <v>4.96E-3</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1694" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1694" t="s">
+        <v>31</v>
+      </c>
       <c r="D1694" s="6">
         <v>3</v>
       </c>
@@ -43766,8 +43913,20 @@
       <c r="F1694">
         <v>2.0729999999999998E-2</v>
       </c>
-    </row>
-    <row r="1695" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1694">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="H1694">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1695" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1695" t="s">
+        <v>31</v>
+      </c>
       <c r="D1695" s="6">
         <v>3</v>
       </c>
@@ -43777,8 +43936,20 @@
       <c r="F1695">
         <v>2.486E-2</v>
       </c>
-    </row>
-    <row r="1696" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G1695">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="H1695">
+        <v>4.8300000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1696" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1696" t="s">
+        <v>31</v>
+      </c>
       <c r="D1696" s="6">
         <v>4</v>
       </c>
@@ -43788,8 +43959,20 @@
       <c r="F1696">
         <v>1.5650000000000001E-2</v>
       </c>
-    </row>
-    <row r="1697" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1696">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H1696">
+        <v>2.4399999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1697" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1697" t="s">
+        <v>31</v>
+      </c>
       <c r="D1697" s="6">
         <v>4</v>
       </c>
@@ -43799,8 +43982,20 @@
       <c r="F1697">
         <v>1.8780000000000002E-2</v>
       </c>
-    </row>
-    <row r="1698" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1697">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="H1697">
+        <v>2.96E-3</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1698" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1698" t="s">
+        <v>31</v>
+      </c>
       <c r="D1698" s="6">
         <v>5</v>
       </c>
@@ -43810,8 +44005,20 @@
       <c r="F1698">
         <v>1.392E-2</v>
       </c>
-    </row>
-    <row r="1699" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1698">
+        <v>0.71</v>
+      </c>
+      <c r="H1698">
+        <v>2.7100000000000002E-3</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1699" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1699" t="s">
+        <v>31</v>
+      </c>
       <c r="D1699" s="6">
         <v>5</v>
       </c>
@@ -43821,8 +44028,20 @@
       <c r="F1699">
         <v>2.0240000000000001E-2</v>
       </c>
-    </row>
-    <row r="1700" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1699">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="H1699">
+        <v>3.5699999999999998E-3</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1700" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1700" t="s">
+        <v>63</v>
+      </c>
       <c r="D1700" s="6">
         <v>6</v>
       </c>
@@ -43832,8 +44051,20 @@
       <c r="F1700">
         <v>0.13361000000000001</v>
       </c>
-    </row>
-    <row r="1701" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1700">
+        <v>5.19</v>
+      </c>
+      <c r="H1700">
+        <v>2.5610000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1701" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1701" t="s">
+        <v>63</v>
+      </c>
       <c r="D1701" s="6">
         <v>6</v>
       </c>
@@ -43843,8 +44074,20 @@
       <c r="F1701">
         <v>0.13702</v>
       </c>
-    </row>
-    <row r="1702" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1701">
+        <v>4.9420000000000002</v>
+      </c>
+      <c r="H1701">
+        <v>2.4219999999999998E-2</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1702" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1702" t="s">
+        <v>63</v>
+      </c>
       <c r="D1702" s="6">
         <v>7</v>
       </c>
@@ -43854,8 +44097,20 @@
       <c r="F1702">
         <v>5.0270000000000002E-2</v>
       </c>
-    </row>
-    <row r="1703" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1702">
+        <v>2.363</v>
+      </c>
+      <c r="H1702">
+        <v>1.133E-2</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1703" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1703" t="s">
+        <v>63</v>
+      </c>
       <c r="D1703" s="6">
         <v>7</v>
       </c>
@@ -43865,8 +44120,20 @@
       <c r="F1703">
         <v>5.1110000000000003E-2</v>
       </c>
-    </row>
-    <row r="1704" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1703">
+        <v>2.4390000000000001</v>
+      </c>
+      <c r="H1703">
+        <v>1.094E-2</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1704" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>63</v>
+      </c>
       <c r="D1704" s="6">
         <v>8</v>
       </c>
@@ -43876,8 +44143,20 @@
       <c r="F1704">
         <v>0.10385</v>
       </c>
-    </row>
-    <row r="1705" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1704">
+        <v>7.5270000000000001</v>
+      </c>
+      <c r="H1704">
+        <v>1.95E-2</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1705" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>63</v>
+      </c>
       <c r="D1705" s="6">
         <v>8</v>
       </c>
@@ -43887,8 +44166,20 @@
       <c r="F1705">
         <v>0.10159</v>
       </c>
-    </row>
-    <row r="1706" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1705">
+        <v>3.3919999999999999</v>
+      </c>
+      <c r="H1705">
+        <v>2.0140000000000002E-2</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1706" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>63</v>
+      </c>
       <c r="D1706" s="6">
         <v>9</v>
       </c>
@@ -43898,8 +44189,20 @@
       <c r="F1706">
         <v>6.3439999999999996E-2</v>
       </c>
-    </row>
-    <row r="1707" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1706">
+        <v>3.2360000000000002</v>
+      </c>
+      <c r="H1706">
+        <v>1.2959999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1707" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>63</v>
+      </c>
       <c r="D1707" s="6">
         <v>9</v>
       </c>
@@ -43909,8 +44212,20 @@
       <c r="F1707">
         <v>6.9839999999999999E-2</v>
       </c>
-    </row>
-    <row r="1708" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1707">
+        <v>3.3919999999999999</v>
+      </c>
+      <c r="H1707">
+        <v>1.2710000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1708" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>63</v>
+      </c>
       <c r="D1708" s="6">
         <v>10</v>
       </c>
@@ -43920,8 +44235,20 @@
       <c r="F1708">
         <v>0.128</v>
       </c>
-    </row>
-    <row r="1709" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1708">
+        <v>5.2350000000000003</v>
+      </c>
+      <c r="H1708">
+        <v>2.317E-2</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1709" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>63</v>
+      </c>
       <c r="D1709" s="6">
         <v>10</v>
       </c>
@@ -43931,135 +44258,324 @@
       <c r="F1709">
         <v>0.10176</v>
       </c>
-    </row>
-    <row r="1710" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="G1709">
+        <v>4.6420000000000003</v>
+      </c>
+      <c r="H1709">
+        <v>2.179E-2</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1710" t="s">
+        <v>9</v>
+      </c>
       <c r="D1710" s="6">
         <v>11</v>
       </c>
       <c r="E1710" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1711" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F1710">
+        <v>7.5259999999999994E-2</v>
+      </c>
+      <c r="G1710">
+        <v>3.5870000000000002</v>
+      </c>
+      <c r="H1710">
+        <v>1.5699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D1711" s="6">
         <v>11</v>
       </c>
       <c r="E1711" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1712" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F1711">
+        <v>8.2979999999999998E-2</v>
+      </c>
+      <c r="G1711">
+        <v>3.9169999999999998</v>
+      </c>
+      <c r="H1711">
+        <v>1.6029999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D1712" s="6">
         <v>12</v>
       </c>
       <c r="E1712" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1713" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1712">
+        <v>0.10551000000000001</v>
+      </c>
+      <c r="G1712">
+        <v>5.1550000000000002</v>
+      </c>
+      <c r="H1712">
+        <v>2.0959999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1713" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1713" s="6">
         <v>12</v>
       </c>
       <c r="E1713" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1714" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1713">
+        <v>0.14854999999999999</v>
+      </c>
+      <c r="G1713">
+        <v>6.8550000000000004</v>
+      </c>
+      <c r="H1713">
+        <v>2.691E-2</v>
+      </c>
+    </row>
+    <row r="1714" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1714" s="6">
         <v>13</v>
       </c>
       <c r="E1714" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1715" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1714">
+        <v>3.9269999999999999E-2</v>
+      </c>
+      <c r="G1714">
+        <v>2.109</v>
+      </c>
+      <c r="H1714">
+        <v>7.9600000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1715" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1715" s="6">
         <v>13</v>
       </c>
       <c r="E1715" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1716" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1715">
+        <v>6.7089999999999997E-2</v>
+      </c>
+      <c r="G1715">
+        <v>3.0419999999999998</v>
+      </c>
+      <c r="H1715">
+        <v>1.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1716" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1716" s="8">
         <v>14</v>
       </c>
       <c r="E1716" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1717" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1716">
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="G1716">
+        <v>4.4379999999999997</v>
+      </c>
+      <c r="H1716">
+        <v>1.7250000000000001E-2</v>
+      </c>
+    </row>
+    <row r="1717" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1717" s="8">
         <v>14</v>
       </c>
       <c r="E1717" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1718" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1717">
+        <v>0.17316000000000001</v>
+      </c>
+      <c r="G1717">
+        <v>5.9950000000000001</v>
+      </c>
+      <c r="H1717">
+        <v>2.9309999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1718" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1718" s="8">
         <v>15</v>
       </c>
       <c r="E1718" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1719" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1718">
+        <v>0.10885</v>
+      </c>
+      <c r="G1718">
+        <v>4.1189999999999998</v>
+      </c>
+      <c r="H1718">
+        <v>1.975E-2</v>
+      </c>
+    </row>
+    <row r="1719" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1719" s="8">
         <v>15</v>
       </c>
       <c r="E1719" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="1720" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1719">
+        <v>6.6259999999999999E-2</v>
+      </c>
+      <c r="G1719">
+        <v>2.9929999999999999</v>
+      </c>
+      <c r="H1719">
+        <v>1.251E-2</v>
+      </c>
+    </row>
+    <row r="1720" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1720" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="1721" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1720">
+        <v>6.0220000000000003E-2</v>
+      </c>
+      <c r="G1720">
+        <v>2.766</v>
+      </c>
+      <c r="H1720">
+        <v>1.193E-2</v>
+      </c>
+    </row>
+    <row r="1721" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1721" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="1722" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1721">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="G1721">
+        <v>3.4239999999999999</v>
+      </c>
+      <c r="H1721">
+        <v>1.401E-2</v>
+      </c>
+    </row>
+    <row r="1722" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1722" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="1723" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1722">
+        <v>0.13911000000000001</v>
+      </c>
+      <c r="G1722">
+        <v>6.085</v>
+      </c>
+      <c r="H1722">
+        <v>2.0820000000000002E-2</v>
+      </c>
+    </row>
+    <row r="1723" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1723" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="1724" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1723">
+        <v>0.11248</v>
+      </c>
+      <c r="G1723">
+        <v>5.1980000000000004</v>
+      </c>
+      <c r="H1723">
+        <v>1.8939999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1724" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1724" s="6">
         <v>18</v>
       </c>
-    </row>
-    <row r="1725" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1724">
+        <v>0.10992</v>
+      </c>
+      <c r="G1724">
+        <v>4.8109999999999999</v>
+      </c>
+      <c r="H1724">
+        <v>1.9619999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1725" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1725" s="6">
         <v>18</v>
       </c>
-    </row>
-    <row r="1726" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1725">
+        <v>0.10942</v>
+      </c>
+      <c r="G1725">
+        <v>4.391</v>
+      </c>
+      <c r="H1725">
+        <v>1.652E-2</v>
+      </c>
+    </row>
+    <row r="1726" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1726" s="6">
         <v>19</v>
       </c>
-    </row>
-    <row r="1727" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1726">
+        <v>7.0550000000000002E-2</v>
+      </c>
+      <c r="G1726">
+        <v>2.8180000000000001</v>
+      </c>
+      <c r="H1726">
+        <v>1.323E-2</v>
+      </c>
+    </row>
+    <row r="1727" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1727" s="6">
         <v>19</v>
       </c>
-    </row>
-    <row r="1728" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F1727">
+        <v>8.1720000000000001E-2</v>
+      </c>
+      <c r="G1727">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="H1727">
+        <v>1.4749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="1728" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1728" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="1729" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="F1728">
+        <v>7.6079999999999995E-2</v>
+      </c>
+      <c r="G1728">
+        <v>3.738</v>
+      </c>
+      <c r="H1728">
+        <v>1.469E-2</v>
+      </c>
+    </row>
+    <row r="1729" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D1729" s="6">
         <v>20</v>
+      </c>
+      <c r="F1729">
+        <v>5.722E-2</v>
+      </c>
+      <c r="G1729">
+        <v>2.9359999999999999</v>
+      </c>
+      <c r="H1729">
+        <v>1.102E-2</v>
       </c>
     </row>
   </sheetData>
@@ -44069,10 +44585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F725AC8B-7FAE-884A-9736-FC083C75F3B8}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44349,7 +44865,7 @@
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -44366,7 +44882,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -44383,7 +44899,7 @@
         <v>3.95E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -44400,7 +44916,7 @@
         <v>3.5200000000000002E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -44417,7 +44933,7 @@
         <v>3.9300000000000002E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -44434,7 +44950,7 @@
         <v>4.19E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -44451,7 +44967,7 @@
         <v>3.49E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -44468,7 +44984,7 @@
         <v>5.9900000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -44479,13 +44995,28 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24">
-        <v>4.58E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -44502,7 +45033,7 @@
         <v>7.1099999999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -44519,7 +45050,7 @@
         <v>4.3299999999999998E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -44536,7 +45067,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -44553,7 +45084,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -44570,7 +45101,7 @@
         <v>6.6799999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -44587,7 +45118,7 @@
         <v>5.7200000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -44604,7 +45135,7 @@
         <v>3.9600000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>

</xml_diff>